<commit_message>
Add Maneuvering Speed Vs. Weight chart for Lance
</commit_message>
<xml_diff>
--- a/pa-32rt-300/pa-32rt-300.xlsx
+++ b/pa-32rt-300/pa-32rt-300.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-32rt-300/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A9EB67-349B-8A4E-A561-E043025B13AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0009B8-1C19-CB4A-8281-587BE2845DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="28160" windowHeight="15360" xr2:uid="{4A64165E-2634-184F-858D-C1C4028D4AFE}"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="15360" activeTab="1" xr2:uid="{4A64165E-2634-184F-858D-C1C4028D4AFE}"/>
   </bookViews>
   <sheets>
     <sheet name="KIAS Vs. % Power " sheetId="1" r:id="rId1"/>
+    <sheet name="Maneuvering Speed Vs. Weight" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Percent Power</t>
   </si>
   <si>
     <t>KIAS</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -606,6 +610,400 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:rPr>
+              <a:t>Maneuvering Speed Vs. Weight</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.281120385060318"/>
+          <c:y val="6.085487664022747E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.8306453225946247E-2"/>
+          <c:y val="0.19618456294903228"/>
+          <c:w val="0.91603312287064875"/>
+          <c:h val="0.77220754326797125"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>KIAS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:backward val="0.5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.740160297313605E-4"/>
+                  <c:y val="0.23550941427649988"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Maneuvering Speed Vs. Weight'!$A$2:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Maneuvering Speed Vs. Weight'!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A300-C84A-A977-F383ABE11C10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="951141263"/>
+        <c:axId val="948993503"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="951141263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3700"/>
+          <c:min val="2100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="948993503"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="948993503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="135"/>
+          <c:min val="110"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="951141263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -646,7 +1044,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1293,6 +2247,49 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>169818</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>189844</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{900A4A11-C832-7043-9F36-1FF421BD6A3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1594,8 +2591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C142E344-91EC-9149-B4F3-7F6FBDA0E0C6}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1651,6 +2648,47 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65282507-3A62-6A4F-9770-20894F5025EA}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3600</v>
+      </c>
+      <c r="B2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2188</v>
+      </c>
+      <c r="B3">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PA-32RT-300: Add Altitude Vs. KCAS
</commit_message>
<xml_diff>
--- a/pa-32rt-300/pa-32rt-300.xlsx
+++ b/pa-32rt-300/pa-32rt-300.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-32rt-300/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0009B8-1C19-CB4A-8281-587BE2845DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF5DA60-30CD-E044-AF51-8DC065344A64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="15360" activeTab="1" xr2:uid="{4A64165E-2634-184F-858D-C1C4028D4AFE}"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="15360" activeTab="2" xr2:uid="{4A64165E-2634-184F-858D-C1C4028D4AFE}"/>
   </bookViews>
   <sheets>
     <sheet name="KIAS Vs. % Power " sheetId="1" r:id="rId1"/>
     <sheet name="Maneuvering Speed Vs. Weight" sheetId="2" r:id="rId2"/>
+    <sheet name="Altitude Vs. KCAS" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Percent Power</t>
   </si>
@@ -43,6 +47,21 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>Pressure Altitude</t>
+  </si>
+  <si>
+    <t>65% Power</t>
+  </si>
+  <si>
+    <t>75% Power</t>
+  </si>
+  <si>
+    <t>KTAS (65%)</t>
+  </si>
+  <si>
+    <t>KTAS (75%)</t>
   </si>
 </sst>
 </file>
@@ -86,10 +105,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -272,84 +292,10 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.9270089444514746E-4"/>
-                  <c:y val="0.1609777875748801"/>
+                  <c:x val="5.6075633796933075E-2"/>
+                  <c:y val="0.22171800337670611"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="900" b="1" i="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                        <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                      </a:rPr>
-                      <a:t>y = -168.73x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="900" b="1" i="0" baseline="30000">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                        <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                      </a:rPr>
-                      <a:t>2</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="900" b="1" i="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                        <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                      </a:rPr>
-                      <a:t> + 344.68x - 17.641</a:t>
-                    </a:r>
-                    <a:br>
-                      <a:rPr lang="en-US" sz="900" b="1" i="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                        <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                      </a:rPr>
-                    </a:br>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="900" b="1" i="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                        <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                      </a:rPr>
-                      <a:t>R² = 1</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="900" b="1" i="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                      <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -395,9 +341,6 @@
                 <c:pt idx="3">
                   <c:v>0.55000000000000004</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.43330000000000002</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -407,6 +350,9 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>166</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>146</c:v>
                 </c:pt>
@@ -415,9 +361,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -444,10 +387,11 @@
         <c:axId val="951141263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="t"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -462,6 +406,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -497,16 +455,17 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="948993503"/>
-        <c:crosses val="max"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5.000000000000001E-2"/>
+        <c:majorUnit val="0.1"/>
+        <c:minorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="948993503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="160"/>
-          <c:min val="50"/>
+          <c:max val="170"/>
+          <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -524,6 +483,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -561,8 +534,8 @@
         <c:crossAx val="951141263"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
-        <c:minorUnit val="2"/>
+        <c:majorUnit val="10"/>
+        <c:minorUnit val="5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -623,6 +596,7 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1004,6 +978,530 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Pressure Altitude Vs. Calibrated Airspeed</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" b="0" i="0">
+                <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:rPr>
+              <a:t>Standard Day (ISA), Peak EGT, 2400 RPM, 3600 lbs.</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.8306453225946247E-2"/>
+          <c:y val="0.19618456294903228"/>
+          <c:w val="0.91603312287064875"/>
+          <c:h val="0.77220754326797125"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Altitude Vs. KCAS'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>75% Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050"/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS'!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>141.99799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>141.81899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>139.59200000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140.07</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ABC5-5F42-9248-AEAE42FEB843}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Altitude Vs. KCAS'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>65% Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>132.99799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>131.126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>129.20099999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>129.05799999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>126.087</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>124.852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ABC5-5F42-9248-AEAE42FEB843}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="951141263"/>
+        <c:axId val="948993503"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="951141263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="85000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="948993503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2000"/>
+        <c:minorUnit val="1000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="948993503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="85000"/>
+              </a:sysClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="951141263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0">
+              <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2217,7 +2715,7 @@
               <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
               <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
             </a:rPr>
-            <a:t> Power Mixture, 3600 lbs. Gross Weight, 2400 RPM, Sea Level, 59</a:t>
+            <a:t> Power Mixture, 3600 lbs. Gross Weight, Sea Level, 59</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" b="1" i="0">
@@ -2290,6 +2788,211 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>254002</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>461820</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>43076</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D8976CD-385D-D640-B2A2-9E79046D18FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="KCAS Vs. % Power (Best Power)"/>
+      <sheetName val="KCAS Vs. % Power (Best Eco)"/>
+      <sheetName val="Altitude Vs. KCAS"/>
+      <sheetName val="Altitude Vs. KCAS (No Fairings)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>65% Power</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>75% Power</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>0</v>
+          </cell>
+          <cell r="B2">
+            <v>107.498</v>
+          </cell>
+          <cell r="C2">
+            <v>114.998</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>1000</v>
+          </cell>
+          <cell r="B3">
+            <v>107.176</v>
+          </cell>
+          <cell r="C3">
+            <v>114.32299999999999</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>2000</v>
+          </cell>
+          <cell r="B4">
+            <v>106.831</v>
+          </cell>
+          <cell r="C4">
+            <v>114.119</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>3000</v>
+          </cell>
+          <cell r="B5">
+            <v>106.462</v>
+          </cell>
+          <cell r="C5">
+            <v>114.24299999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>4000</v>
+          </cell>
+          <cell r="B6">
+            <v>106.07</v>
+          </cell>
+          <cell r="C6">
+            <v>113.739</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>5000</v>
+          </cell>
+          <cell r="B7">
+            <v>105.65600000000001</v>
+          </cell>
+          <cell r="C7">
+            <v>113.21299999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>6000</v>
+          </cell>
+          <cell r="B8">
+            <v>105.21899999999999</v>
+          </cell>
+          <cell r="C8">
+            <v>112.551</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>7000</v>
+          </cell>
+          <cell r="B9">
+            <v>104.761</v>
+          </cell>
+          <cell r="C9">
+            <v>112.663</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>8000</v>
+          </cell>
+          <cell r="B10">
+            <v>104.193</v>
+          </cell>
+          <cell r="C10">
+            <v>112.066</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>9000</v>
+          </cell>
+          <cell r="B11">
+            <v>103.563</v>
+          </cell>
+          <cell r="C11">
+            <v>111.45</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>10000</v>
+          </cell>
+          <cell r="B12">
+            <v>102.83</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>11000</v>
+          </cell>
+          <cell r="B13">
+            <v>102.084</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>12000</v>
+          </cell>
+          <cell r="B14">
+            <v>101.324</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2587,12 +3290,584 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C142E344-91EC-9149-B4F3-7F6FBDA0E0C6}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A3" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2601,7 +3876,7 @@
     <col min="2" max="2" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2609,42 +3884,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
+      <c r="B2" s="2">
+        <v>166</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.75</v>
       </c>
       <c r="B3" s="2">
         <v>146</v>
       </c>
+      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.65</v>
       </c>
       <c r="B4" s="2">
         <v>135</v>
       </c>
+      <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.55000000000000004</v>
       </c>
       <c r="B5" s="2">
         <v>121</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>0.43330000000000002</v>
-      </c>
-      <c r="B6" s="2">
-        <v>100</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2657,7 +3931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65282507-3A62-6A4F-9770-20894F5025EA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2691,4 +3965,166 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A944C1F-B5C8-BC42-BED6-C9445F0DAC7A}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>132.99799999999999</v>
+      </c>
+      <c r="C2">
+        <v>141.99799999999999</v>
+      </c>
+      <c r="D2">
+        <v>133</v>
+      </c>
+      <c r="E2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>131.126</v>
+      </c>
+      <c r="C4">
+        <v>141.81899999999999</v>
+      </c>
+      <c r="D4">
+        <v>135</v>
+      </c>
+      <c r="E4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4000</v>
+      </c>
+      <c r="B6">
+        <v>129.20099999999999</v>
+      </c>
+      <c r="C6">
+        <v>139.59200000000001</v>
+      </c>
+      <c r="D6">
+        <v>137</v>
+      </c>
+      <c r="E6">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6000</v>
+      </c>
+      <c r="B8">
+        <v>129.05799999999999</v>
+      </c>
+      <c r="C8">
+        <v>140.07</v>
+      </c>
+      <c r="D8">
+        <v>141</v>
+      </c>
+      <c r="E8">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8000</v>
+      </c>
+      <c r="B10">
+        <v>126.087</v>
+      </c>
+      <c r="D10">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10000</v>
+      </c>
+      <c r="B12">
+        <v>124.852</v>
+      </c>
+      <c r="D12">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>